<commit_message>
listas de cadastro de usuário PM/PC
</commit_message>
<xml_diff>
--- a/cad_user/USUARIOS CONFIRMADOS IMEIGUARD.xlsx
+++ b/cad_user/USUARIOS CONFIRMADOS IMEIGUARD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DEAC_TI_SW\Users\DEAC_TI_SERVER\Desktop\IMEIGuardWEB\cad_user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DEAC_TI_SW\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963605FA-471C-407C-B25E-70A0178DDCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C1D78C-2028-4CA5-A898-459FB77937BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D5B3F50-1031-4000-A71D-A098494E9EE1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D5B3F50-1031-4000-A71D-A098494E9EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="1027">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -2766,6 +2766,360 @@
   </si>
   <si>
     <t>leonidas.donza@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>fabriciosozar123@gmail.com</t>
+  </si>
+  <si>
+    <t>FABRICIO RODRIGUES SOZAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPC </t>
+  </si>
+  <si>
+    <t>SECCIONAL DA CIDADE NOVA</t>
+  </si>
+  <si>
+    <t>fabricio.sozar@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>felipe.soares@lers.google</t>
+  </si>
+  <si>
+    <t>FELIPE MATHEUS RIBEIRO JUCA SOARES</t>
+  </si>
+  <si>
+    <t>01378726235</t>
+  </si>
+  <si>
+    <t>SECCIONAL DO COMERCIO DE BELEM</t>
+  </si>
+  <si>
+    <t>felipe.soares@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>jeallysonfreitas@gmail.com</t>
+  </si>
+  <si>
+    <t>ANTONIO JEALLYSON DE FREITAS PEREIRA</t>
+  </si>
+  <si>
+    <t>06571021307</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE HOMICIDIOS DE TUCURUI</t>
+  </si>
+  <si>
+    <t>antonio.pereira@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>jocemir_bastos@hotmail.com</t>
+  </si>
+  <si>
+    <t>JOCEMIR BASTOS DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jocemir_bastos@hotmail.com </t>
+  </si>
+  <si>
+    <t>vitormarcelinobcosta@gmail.com</t>
+  </si>
+  <si>
+    <t>VITOR MARCELINO BORGES COSTA</t>
+  </si>
+  <si>
+    <t>01983304301</t>
+  </si>
+  <si>
+    <t>ICUI-GUAJARA</t>
+  </si>
+  <si>
+    <t>vitor.borges@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>bentesnogueira@gmail.com</t>
+  </si>
+  <si>
+    <t>WILLIAM BENTES NOGUEIRA</t>
+  </si>
+  <si>
+    <t>william.nogueira@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>denysrodrigues1987@gmail.com</t>
+  </si>
+  <si>
+    <t>DENYS RODRIGUES BORGES MARINHO</t>
+  </si>
+  <si>
+    <t>01855091348</t>
+  </si>
+  <si>
+    <t>ULIANOPOLIS-PA</t>
+  </si>
+  <si>
+    <t>denys.marinho@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>elizabethgferraz@hotmail.com</t>
+  </si>
+  <si>
+    <t>ELIZABETH GARCIA CAVALLEIRO DE MACEDO FERRAZ</t>
+  </si>
+  <si>
+    <t>SECCIONAL URBANA DO COMERCIO</t>
+  </si>
+  <si>
+    <t>elizabeth.ferraz@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>ivaniltonnunes897@gmail.com</t>
+  </si>
+  <si>
+    <t>IVANILTON MONTEIRO NUNES</t>
+  </si>
+  <si>
+    <t>UISP SAO FELIX-MARABA/PA</t>
+  </si>
+  <si>
+    <t>ivanilton.nunes@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>carolina.morgana@gmail.com</t>
+  </si>
+  <si>
+    <t>CAROLINA MORGANA FRANCA PAMPLONA</t>
+  </si>
+  <si>
+    <t>carolina.pamplona@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>rocaro4102@gmail.com</t>
+  </si>
+  <si>
+    <t>RODOLFO CARVALHO ROCHA</t>
+  </si>
+  <si>
+    <t>00174550308</t>
+  </si>
+  <si>
+    <t>UNIDADE INTEGRADA DE SEGURANCA PUBLICA - UISP SAO FELIX - MARABA/PA.</t>
+  </si>
+  <si>
+    <t>rodolfo.rocha@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>delegaciamagalhaesbarata@gmail.com</t>
+  </si>
+  <si>
+    <t>DIEGO RODRIGO FIGUEIREDO PINHEIRO</t>
+  </si>
+  <si>
+    <t>MUNICIPIO DE MAGALHAES BARATA-DPI</t>
+  </si>
+  <si>
+    <t>diego.pinheiro@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>eldermonteiro.odonto@gmail.com</t>
+  </si>
+  <si>
+    <t>ELDER MONTEIRO DO NASCIMENTO</t>
+  </si>
+  <si>
+    <t>DIVISAO DE HOMICIDIO</t>
+  </si>
+  <si>
+    <t>elder.nascimento@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>tadeuguilhonescrivao@gmail.com</t>
+  </si>
+  <si>
+    <t>JORGE TADEU DO ESPIRITO SANTO GUILHON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">271.444.022-34 </t>
+  </si>
+  <si>
+    <t>DIVISAO DE HOMICIDIOS</t>
+  </si>
+  <si>
+    <t>suellensousaconcurseira@gmail.com</t>
+  </si>
+  <si>
+    <t>SUELLEN CARVALHO DE SOUZA MELO</t>
+  </si>
+  <si>
+    <t>marcosvfm00@gmail.com</t>
+  </si>
+  <si>
+    <t>MARCUS VINICIUS FILGUEIRAS MATOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">629.206.692-49 </t>
+  </si>
+  <si>
+    <t>marcus.matos@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>alcineymb@gmail.com</t>
+  </si>
+  <si>
+    <t>ALCINEY MODESTO BRAGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">423.000.292-00 </t>
+  </si>
+  <si>
+    <t>alcineymb@hotmail.com</t>
+  </si>
+  <si>
+    <t>f_mileo@hotmail.com</t>
+  </si>
+  <si>
+    <t>FELIPE MILEO DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>00597055238</t>
+  </si>
+  <si>
+    <t>felipe.almeida@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>nilsonramosipc@gmail.com</t>
+  </si>
+  <si>
+    <t>NILSON JOSE DE SOUZA RAMOS</t>
+  </si>
+  <si>
+    <t>DH/ ICOARACI</t>
+  </si>
+  <si>
+    <t>murillo.monteiro.pf3@gmail.com</t>
+  </si>
+  <si>
+    <t>MURILLO DE OLIVEIRA MONTEIRO</t>
+  </si>
+  <si>
+    <t>danielipcdpe@gmail.com</t>
+  </si>
+  <si>
+    <t>DANIEL FARO LOBATO</t>
+  </si>
+  <si>
+    <t>02579762213</t>
+  </si>
+  <si>
+    <t>daniel.lobato@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>jhonpavly96@gmail.com</t>
+  </si>
+  <si>
+    <t>JONATHAN MATEUS DA SILVA</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE VITORIA DO XINGU</t>
+  </si>
+  <si>
+    <t>jonathan.mateus@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>jorgefielpc@gmail.com</t>
+  </si>
+  <si>
+    <t>JORGE LUIS FIEL DE FARIAS</t>
+  </si>
+  <si>
+    <t>jorge.farias@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>brunorito@hotmail.com</t>
+  </si>
+  <si>
+    <t>BRUNO RITO COSME DA SILVA</t>
+  </si>
+  <si>
+    <t>CAF-DRCO</t>
+  </si>
+  <si>
+    <t>bruno.rito@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>fabner.gomes.2015@gmail.com</t>
+  </si>
+  <si>
+    <t>FABNER GOMES DA SILVA</t>
+  </si>
+  <si>
+    <t>04140325437</t>
+  </si>
+  <si>
+    <t>NAI TUCURUÍ</t>
+  </si>
+  <si>
+    <t>fabner.silva@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>macedoneto90@gmail.com</t>
+  </si>
+  <si>
+    <t>ANTONIO DE SOUSA MACEDO NETO</t>
+  </si>
+  <si>
+    <t>antonio.macedo@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>gustavorocha1069@gmail.com</t>
+  </si>
+  <si>
+    <t>gustavo.arantes@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>narabensantos@gmail.com</t>
+  </si>
+  <si>
+    <t>nara.santos@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>OUREM</t>
+  </si>
+  <si>
+    <t>XINGUARA</t>
+  </si>
+  <si>
+    <t>GUSTAVO ARANTES ROCHA</t>
+  </si>
+  <si>
+    <t>NARA BENEDITA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>MAGALHAES BARATA</t>
+  </si>
+  <si>
+    <t>6/27/2024 14:35:13</t>
+  </si>
+  <si>
+    <t>6/27/2024 15:52:25</t>
+  </si>
+  <si>
+    <t>6/27/2024 16:47:52</t>
+  </si>
+  <si>
+    <t>6/28/2024 16:25:03</t>
+  </si>
+  <si>
+    <t>natanpedrosa13@outlook.com</t>
+  </si>
+  <si>
+    <t>NATAN FLAVIO PEDROSA</t>
+  </si>
+  <si>
+    <t>19° SECCIONAL DE POLICIA CIVIL DE ITAITUBA</t>
+  </si>
+  <si>
+    <t>natan.pedrosa@policiacivil.pa.gov.br</t>
   </si>
 </sst>
 </file>
@@ -2775,7 +3129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2818,6 +3172,28 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2855,7 +3231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2888,6 +3264,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3224,21 +3606,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F6D7D1-5711-44E6-A7F2-3BDEABEFDFB8}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:O280"/>
+  <dimension ref="A1:O283"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A247" sqref="A247:XFD253"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A282" sqref="A282:J282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="5"/>
     <col min="2" max="2" width="35.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="20.7109375" style="5"/>
     <col min="8" max="8" width="67.5703125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="20.7109375" style="5"/>
+    <col min="9" max="9" width="43.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="20.7109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -12559,21 +12942,41 @@
       <c r="I253" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="J253" t="s">
+      <c r="J253" s="14" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A254" s="4"/>
-      <c r="B254" s="4"/>
-      <c r="C254" s="4"/>
-      <c r="D254" s="4"/>
-      <c r="E254" s="4"/>
-      <c r="F254" s="4"/>
-      <c r="G254" s="4"/>
-      <c r="H254" s="4"/>
-      <c r="I254" s="4"/>
-      <c r="J254" s="4"/>
+      <c r="A254" s="13">
+        <v>45467.494538599538</v>
+      </c>
+      <c r="B254" s="11" t="s">
+        <v>909</v>
+      </c>
+      <c r="C254" s="11" t="s">
+        <v>910</v>
+      </c>
+      <c r="D254" s="11">
+        <v>57199987</v>
+      </c>
+      <c r="E254" s="11">
+        <v>86180800200</v>
+      </c>
+      <c r="F254" s="11" t="s">
+        <v>911</v>
+      </c>
+      <c r="G254" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H254" s="11" t="s">
+        <v>912</v>
+      </c>
+      <c r="I254" s="11" t="s">
+        <v>913</v>
+      </c>
+      <c r="J254" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K254" s="4"/>
       <c r="L254" s="4"/>
       <c r="M254" s="4"/>
@@ -12581,16 +12984,36 @@
       <c r="O254" s="4"/>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A255" s="4"/>
-      <c r="B255" s="4"/>
-      <c r="C255" s="4"/>
-      <c r="D255" s="4"/>
-      <c r="E255" s="4"/>
-      <c r="F255" s="4"/>
-      <c r="G255" s="4"/>
-      <c r="H255" s="4"/>
-      <c r="I255" s="4"/>
-      <c r="J255" s="4"/>
+      <c r="A255" s="13">
+        <v>45467.623150405096</v>
+      </c>
+      <c r="B255" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="C255" s="11" t="s">
+        <v>915</v>
+      </c>
+      <c r="D255" s="11">
+        <v>5909573</v>
+      </c>
+      <c r="E255" s="12" t="s">
+        <v>916</v>
+      </c>
+      <c r="F255" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G255" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H255" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="I255" s="11" t="s">
+        <v>918</v>
+      </c>
+      <c r="J255" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K255" s="4"/>
       <c r="L255" s="4"/>
       <c r="M255" s="4"/>
@@ -12598,16 +13021,36 @@
       <c r="O255" s="4"/>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A256" s="4"/>
-      <c r="B256" s="4"/>
-      <c r="C256" s="4"/>
-      <c r="D256" s="4"/>
-      <c r="E256" s="4"/>
-      <c r="F256" s="4"/>
-      <c r="G256" s="4"/>
-      <c r="H256" s="4"/>
-      <c r="I256" s="4"/>
-      <c r="J256" s="4"/>
+      <c r="A256" s="13">
+        <v>45467.664150416662</v>
+      </c>
+      <c r="B256" s="11" t="s">
+        <v>919</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="D256" s="11">
+        <v>5966684</v>
+      </c>
+      <c r="E256" s="12" t="s">
+        <v>921</v>
+      </c>
+      <c r="F256" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G256" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H256" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="I256" s="11" t="s">
+        <v>923</v>
+      </c>
+      <c r="J256" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K256" s="4"/>
       <c r="L256" s="4"/>
       <c r="M256" s="4"/>
@@ -12615,16 +13058,36 @@
       <c r="O256" s="4"/>
     </row>
     <row r="257" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A257" s="4"/>
-      <c r="B257" s="4"/>
-      <c r="C257" s="4"/>
-      <c r="D257" s="4"/>
-      <c r="E257" s="4"/>
-      <c r="F257" s="4"/>
-      <c r="G257" s="4"/>
-      <c r="H257" s="4"/>
-      <c r="I257" s="4"/>
-      <c r="J257" s="4"/>
+      <c r="A257" s="13">
+        <v>45467.890480347225</v>
+      </c>
+      <c r="B257" s="11" t="s">
+        <v>924</v>
+      </c>
+      <c r="C257" s="11" t="s">
+        <v>925</v>
+      </c>
+      <c r="D257" s="11">
+        <v>8400710</v>
+      </c>
+      <c r="E257" s="11">
+        <v>42624924272</v>
+      </c>
+      <c r="F257" s="11" t="s">
+        <v>911</v>
+      </c>
+      <c r="G257" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H257" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="I257" s="11" t="s">
+        <v>926</v>
+      </c>
+      <c r="J257" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K257" s="4"/>
       <c r="L257" s="4"/>
       <c r="M257" s="4"/>
@@ -12632,16 +13095,36 @@
       <c r="O257" s="4"/>
     </row>
     <row r="258" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A258" s="4"/>
-      <c r="B258" s="4"/>
-      <c r="C258" s="4"/>
-      <c r="D258" s="4"/>
-      <c r="E258" s="4"/>
-      <c r="F258" s="4"/>
-      <c r="G258" s="4"/>
-      <c r="H258" s="4"/>
-      <c r="I258" s="4"/>
-      <c r="J258" s="4"/>
+      <c r="A258" s="13">
+        <v>45468.378864988423</v>
+      </c>
+      <c r="B258" s="11" t="s">
+        <v>927</v>
+      </c>
+      <c r="C258" s="11" t="s">
+        <v>928</v>
+      </c>
+      <c r="D258" s="11">
+        <v>5914026</v>
+      </c>
+      <c r="E258" s="12" t="s">
+        <v>929</v>
+      </c>
+      <c r="F258" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G258" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H258" s="11" t="s">
+        <v>930</v>
+      </c>
+      <c r="I258" s="11" t="s">
+        <v>931</v>
+      </c>
+      <c r="J258" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K258" s="4"/>
       <c r="L258" s="4"/>
       <c r="M258" s="4"/>
@@ -12649,16 +13132,36 @@
       <c r="O258" s="4"/>
     </row>
     <row r="259" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A259" s="4"/>
-      <c r="B259" s="4"/>
-      <c r="C259" s="4"/>
-      <c r="D259" s="4"/>
-      <c r="E259" s="4"/>
-      <c r="F259" s="4"/>
-      <c r="G259" s="4"/>
-      <c r="H259" s="4"/>
-      <c r="I259" s="4"/>
-      <c r="J259" s="4"/>
+      <c r="A259" s="13">
+        <v>45468.484094270832</v>
+      </c>
+      <c r="B259" s="11" t="s">
+        <v>932</v>
+      </c>
+      <c r="C259" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="D259" s="11">
+        <v>57173848</v>
+      </c>
+      <c r="E259" s="11">
+        <v>78813522215</v>
+      </c>
+      <c r="F259" s="11" t="s">
+        <v>911</v>
+      </c>
+      <c r="G259" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H259" s="11" t="s">
+        <v>795</v>
+      </c>
+      <c r="I259" s="11" t="s">
+        <v>934</v>
+      </c>
+      <c r="J259" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K259" s="4"/>
       <c r="L259" s="4"/>
       <c r="M259" s="4"/>
@@ -12666,16 +13169,36 @@
       <c r="O259" s="4"/>
     </row>
     <row r="260" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A260" s="4"/>
-      <c r="B260" s="4"/>
-      <c r="C260" s="4"/>
-      <c r="D260" s="4"/>
-      <c r="E260" s="4"/>
-      <c r="F260" s="4"/>
-      <c r="G260" s="4"/>
-      <c r="H260" s="4"/>
-      <c r="I260" s="4"/>
-      <c r="J260" s="4"/>
+      <c r="A260" s="13">
+        <v>45468.492225717593</v>
+      </c>
+      <c r="B260" s="11" t="s">
+        <v>935</v>
+      </c>
+      <c r="C260" s="11" t="s">
+        <v>936</v>
+      </c>
+      <c r="D260" s="11">
+        <v>5966688</v>
+      </c>
+      <c r="E260" s="12" t="s">
+        <v>937</v>
+      </c>
+      <c r="F260" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G260" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H260" s="11" t="s">
+        <v>938</v>
+      </c>
+      <c r="I260" s="11" t="s">
+        <v>939</v>
+      </c>
+      <c r="J260" s="14" t="s">
+        <v>494</v>
+      </c>
       <c r="K260" s="4"/>
       <c r="L260" s="4"/>
       <c r="M260" s="4"/>
@@ -12683,16 +13206,36 @@
       <c r="O260" s="4"/>
     </row>
     <row r="261" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A261" s="4"/>
-      <c r="B261" s="4"/>
-      <c r="C261" s="4"/>
-      <c r="D261" s="4"/>
-      <c r="E261" s="4"/>
-      <c r="F261" s="4"/>
-      <c r="G261" s="4"/>
-      <c r="H261" s="4"/>
-      <c r="I261" s="4"/>
-      <c r="J261" s="4"/>
+      <c r="A261" s="15">
+        <v>45468.657388263891</v>
+      </c>
+      <c r="B261" s="16" t="s">
+        <v>940</v>
+      </c>
+      <c r="C261" s="16" t="s">
+        <v>941</v>
+      </c>
+      <c r="D261" s="16">
+        <v>5966708</v>
+      </c>
+      <c r="E261" s="16">
+        <v>47988053272</v>
+      </c>
+      <c r="F261" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G261" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H261" s="16" t="s">
+        <v>942</v>
+      </c>
+      <c r="I261" s="16" t="s">
+        <v>943</v>
+      </c>
+      <c r="J261" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K261" s="4"/>
       <c r="L261" s="4"/>
       <c r="M261" s="4"/>
@@ -12700,16 +13243,36 @@
       <c r="O261" s="4"/>
     </row>
     <row r="262" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A262" s="4"/>
-      <c r="B262" s="4"/>
-      <c r="C262" s="4"/>
-      <c r="D262" s="4"/>
-      <c r="E262" s="4"/>
-      <c r="F262" s="4"/>
-      <c r="G262" s="4"/>
-      <c r="H262" s="4"/>
-      <c r="I262" s="4"/>
-      <c r="J262" s="4"/>
+      <c r="A262" s="15">
+        <v>45468.669052094905</v>
+      </c>
+      <c r="B262" s="16" t="s">
+        <v>944</v>
+      </c>
+      <c r="C262" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="D262" s="16">
+        <v>57222128</v>
+      </c>
+      <c r="E262" s="16">
+        <v>96290463268</v>
+      </c>
+      <c r="F262" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G262" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H262" s="16" t="s">
+        <v>946</v>
+      </c>
+      <c r="I262" s="16" t="s">
+        <v>947</v>
+      </c>
+      <c r="J262" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K262" s="4"/>
       <c r="L262" s="4"/>
       <c r="M262" s="4"/>
@@ -12717,16 +13280,36 @@
       <c r="O262" s="4"/>
     </row>
     <row r="263" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A263" s="4"/>
-      <c r="B263" s="4"/>
-      <c r="C263" s="4"/>
-      <c r="D263" s="4"/>
-      <c r="E263" s="4"/>
-      <c r="F263" s="4"/>
-      <c r="G263" s="4"/>
-      <c r="H263" s="4"/>
-      <c r="I263" s="4"/>
-      <c r="J263" s="4"/>
+      <c r="A263" s="15">
+        <v>45468.672788217591</v>
+      </c>
+      <c r="B263" s="16" t="s">
+        <v>948</v>
+      </c>
+      <c r="C263" s="16" t="s">
+        <v>949</v>
+      </c>
+      <c r="D263" s="16">
+        <v>5966511</v>
+      </c>
+      <c r="E263" s="16">
+        <v>95205349204</v>
+      </c>
+      <c r="F263" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G263" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H263" s="16" t="s">
+        <v>682</v>
+      </c>
+      <c r="I263" s="16" t="s">
+        <v>950</v>
+      </c>
+      <c r="J263" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K263" s="4"/>
       <c r="L263" s="4"/>
       <c r="M263" s="4"/>
@@ -12734,16 +13317,36 @@
       <c r="O263" s="4"/>
     </row>
     <row r="264" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A264" s="4"/>
-      <c r="B264" s="4"/>
-      <c r="C264" s="4"/>
-      <c r="D264" s="4"/>
-      <c r="E264" s="4"/>
-      <c r="F264" s="4"/>
-      <c r="G264" s="4"/>
-      <c r="H264" s="4"/>
-      <c r="I264" s="4"/>
-      <c r="J264" s="4"/>
+      <c r="A264" s="15">
+        <v>45468.673942534719</v>
+      </c>
+      <c r="B264" s="16" t="s">
+        <v>951</v>
+      </c>
+      <c r="C264" s="16" t="s">
+        <v>952</v>
+      </c>
+      <c r="D264" s="16">
+        <v>5966249</v>
+      </c>
+      <c r="E264" s="18" t="s">
+        <v>953</v>
+      </c>
+      <c r="F264" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G264" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H264" s="16" t="s">
+        <v>954</v>
+      </c>
+      <c r="I264" s="16" t="s">
+        <v>955</v>
+      </c>
+      <c r="J264" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K264" s="4"/>
       <c r="L264" s="4"/>
       <c r="M264" s="4"/>
@@ -12751,16 +13354,36 @@
       <c r="O264" s="4"/>
     </row>
     <row r="265" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A265" s="4"/>
-      <c r="B265" s="4"/>
-      <c r="C265" s="4"/>
-      <c r="D265" s="4"/>
-      <c r="E265" s="4"/>
-      <c r="F265" s="4"/>
-      <c r="G265" s="4"/>
-      <c r="H265" s="4"/>
-      <c r="I265" s="4"/>
-      <c r="J265" s="4"/>
+      <c r="A265" s="15">
+        <v>45468.688992650466</v>
+      </c>
+      <c r="B265" s="16" t="s">
+        <v>956</v>
+      </c>
+      <c r="C265" s="16" t="s">
+        <v>957</v>
+      </c>
+      <c r="D265" s="16">
+        <v>57212799</v>
+      </c>
+      <c r="E265" s="16">
+        <v>53317815272</v>
+      </c>
+      <c r="F265" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G265" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H265" s="16" t="s">
+        <v>958</v>
+      </c>
+      <c r="I265" s="16" t="s">
+        <v>959</v>
+      </c>
+      <c r="J265" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K265" s="4"/>
       <c r="L265" s="4"/>
       <c r="M265" s="4"/>
@@ -12768,16 +13391,36 @@
       <c r="O265" s="4"/>
     </row>
     <row r="266" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A266" s="4"/>
-      <c r="B266" s="4"/>
-      <c r="C266" s="4"/>
-      <c r="D266" s="4"/>
-      <c r="E266" s="4"/>
-      <c r="F266" s="4"/>
-      <c r="G266" s="4"/>
-      <c r="H266" s="4"/>
-      <c r="I266" s="4"/>
-      <c r="J266" s="4"/>
+      <c r="A266" s="15">
+        <v>45468.718717384254</v>
+      </c>
+      <c r="B266" s="16" t="s">
+        <v>960</v>
+      </c>
+      <c r="C266" s="16" t="s">
+        <v>961</v>
+      </c>
+      <c r="D266" s="16">
+        <v>5966636</v>
+      </c>
+      <c r="E266" s="16">
+        <v>78721571287</v>
+      </c>
+      <c r="F266" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G266" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H266" s="16" t="s">
+        <v>962</v>
+      </c>
+      <c r="I266" s="16" t="s">
+        <v>963</v>
+      </c>
+      <c r="J266" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K266" s="4"/>
       <c r="L266" s="4"/>
       <c r="M266" s="4"/>
@@ -12785,16 +13428,36 @@
       <c r="O266" s="4"/>
     </row>
     <row r="267" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A267" s="4"/>
-      <c r="B267" s="4"/>
-      <c r="C267" s="4"/>
-      <c r="D267" s="4"/>
-      <c r="E267" s="4"/>
-      <c r="F267" s="4"/>
-      <c r="G267" s="4"/>
-      <c r="H267" s="4"/>
-      <c r="I267" s="4"/>
-      <c r="J267" s="4"/>
+      <c r="A267" s="15">
+        <v>45468.71998952546</v>
+      </c>
+      <c r="B267" s="16" t="s">
+        <v>964</v>
+      </c>
+      <c r="C267" s="16" t="s">
+        <v>965</v>
+      </c>
+      <c r="D267" s="16">
+        <v>5461731</v>
+      </c>
+      <c r="E267" s="16" t="s">
+        <v>966</v>
+      </c>
+      <c r="F267" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G267" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H267" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="I267" s="16" t="s">
+        <v>964</v>
+      </c>
+      <c r="J267" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K267" s="4"/>
       <c r="L267" s="4"/>
       <c r="M267" s="4"/>
@@ -12802,16 +13465,36 @@
       <c r="O267" s="4"/>
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A268" s="4"/>
-      <c r="B268" s="4"/>
-      <c r="C268" s="4"/>
-      <c r="D268" s="4"/>
-      <c r="E268" s="4"/>
-      <c r="F268" s="4"/>
-      <c r="G268" s="4"/>
-      <c r="H268" s="4"/>
-      <c r="I268" s="4"/>
-      <c r="J268" s="4"/>
+      <c r="A268" s="15">
+        <v>45468.720439293982</v>
+      </c>
+      <c r="B268" s="16" t="s">
+        <v>968</v>
+      </c>
+      <c r="C268" s="16" t="s">
+        <v>969</v>
+      </c>
+      <c r="D268" s="16">
+        <v>57224582</v>
+      </c>
+      <c r="E268" s="16">
+        <v>78689872272</v>
+      </c>
+      <c r="F268" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G268" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H268" s="16" t="s">
+        <v>860</v>
+      </c>
+      <c r="I268" s="16" t="s">
+        <v>968</v>
+      </c>
+      <c r="J268" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K268" s="4"/>
       <c r="L268" s="4"/>
       <c r="M268" s="4"/>
@@ -12819,16 +13502,36 @@
       <c r="O268" s="4"/>
     </row>
     <row r="269" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A269" s="4"/>
-      <c r="B269" s="4"/>
-      <c r="C269" s="4"/>
-      <c r="D269" s="4"/>
-      <c r="E269" s="4"/>
-      <c r="F269" s="4"/>
-      <c r="G269" s="4"/>
-      <c r="H269" s="4"/>
-      <c r="I269" s="4"/>
-      <c r="J269" s="4"/>
+      <c r="A269" s="15">
+        <v>45468.721062881945</v>
+      </c>
+      <c r="B269" s="16" t="s">
+        <v>970</v>
+      </c>
+      <c r="C269" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="D269" s="16">
+        <v>54183825</v>
+      </c>
+      <c r="E269" s="16" t="s">
+        <v>972</v>
+      </c>
+      <c r="F269" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G269" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H269" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="I269" s="16" t="s">
+        <v>973</v>
+      </c>
+      <c r="J269" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K269" s="4"/>
       <c r="L269" s="4"/>
       <c r="M269" s="4"/>
@@ -12836,16 +13539,36 @@
       <c r="O269" s="4"/>
     </row>
     <row r="270" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A270" s="4"/>
-      <c r="B270" s="4"/>
-      <c r="C270" s="4"/>
-      <c r="D270" s="4"/>
-      <c r="E270" s="4"/>
-      <c r="F270" s="4"/>
-      <c r="G270" s="4"/>
-      <c r="H270" s="4"/>
-      <c r="I270" s="4"/>
-      <c r="J270" s="4"/>
+      <c r="A270" s="15">
+        <v>45468.722990104172</v>
+      </c>
+      <c r="B270" s="16" t="s">
+        <v>974</v>
+      </c>
+      <c r="C270" s="16" t="s">
+        <v>975</v>
+      </c>
+      <c r="D270" s="16">
+        <v>54183800</v>
+      </c>
+      <c r="E270" s="16" t="s">
+        <v>976</v>
+      </c>
+      <c r="F270" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G270" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H270" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="I270" s="16" t="s">
+        <v>977</v>
+      </c>
+      <c r="J270" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K270" s="4"/>
       <c r="L270" s="4"/>
       <c r="M270" s="4"/>
@@ -12853,16 +13576,36 @@
       <c r="O270" s="4"/>
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A271" s="4"/>
-      <c r="B271" s="4"/>
-      <c r="C271" s="4"/>
-      <c r="D271" s="4"/>
-      <c r="E271" s="4"/>
-      <c r="F271" s="4"/>
-      <c r="G271" s="4"/>
-      <c r="H271" s="4"/>
-      <c r="I271" s="4"/>
-      <c r="J271" s="4"/>
+      <c r="A271" s="15">
+        <v>45468.724292060186</v>
+      </c>
+      <c r="B271" s="16" t="s">
+        <v>978</v>
+      </c>
+      <c r="C271" s="16" t="s">
+        <v>979</v>
+      </c>
+      <c r="D271" s="16">
+        <v>55209638</v>
+      </c>
+      <c r="E271" s="18" t="s">
+        <v>980</v>
+      </c>
+      <c r="F271" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G271" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H271" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="I271" s="16" t="s">
+        <v>981</v>
+      </c>
+      <c r="J271" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K271" s="4"/>
       <c r="L271" s="4"/>
       <c r="M271" s="4"/>
@@ -12870,16 +13613,36 @@
       <c r="O271" s="4"/>
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A272" s="4"/>
-      <c r="B272" s="4"/>
-      <c r="C272" s="4"/>
-      <c r="D272" s="4"/>
-      <c r="E272" s="4"/>
-      <c r="F272" s="4"/>
-      <c r="G272" s="4"/>
-      <c r="H272" s="4"/>
-      <c r="I272" s="4"/>
-      <c r="J272" s="4"/>
+      <c r="A272" s="15">
+        <v>45468.72643480324</v>
+      </c>
+      <c r="B272" s="16" t="s">
+        <v>982</v>
+      </c>
+      <c r="C272" s="16" t="s">
+        <v>983</v>
+      </c>
+      <c r="D272" s="16">
+        <v>5886694</v>
+      </c>
+      <c r="E272" s="16">
+        <v>43044719291</v>
+      </c>
+      <c r="F272" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G272" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H272" s="16" t="s">
+        <v>984</v>
+      </c>
+      <c r="I272" s="16" t="s">
+        <v>982</v>
+      </c>
+      <c r="J272" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K272" s="4"/>
       <c r="L272" s="4"/>
       <c r="M272" s="4"/>
@@ -12887,16 +13650,36 @@
       <c r="O272" s="4"/>
     </row>
     <row r="273" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A273" s="4"/>
-      <c r="B273" s="4"/>
-      <c r="C273" s="4"/>
-      <c r="D273" s="4"/>
-      <c r="E273" s="4"/>
-      <c r="F273" s="4"/>
-      <c r="G273" s="4"/>
-      <c r="H273" s="4"/>
-      <c r="I273" s="4"/>
-      <c r="J273" s="4"/>
+      <c r="A273" s="15">
+        <v>45468.770018634255</v>
+      </c>
+      <c r="B273" s="16" t="s">
+        <v>985</v>
+      </c>
+      <c r="C273" s="16" t="s">
+        <v>986</v>
+      </c>
+      <c r="D273" s="16">
+        <v>57233575</v>
+      </c>
+      <c r="E273" s="16">
+        <v>71621709272</v>
+      </c>
+      <c r="F273" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G273" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H273" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="I273" s="16" t="s">
+        <v>985</v>
+      </c>
+      <c r="J273" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="K273" s="4"/>
       <c r="L273" s="4"/>
       <c r="M273" s="4"/>
@@ -12904,16 +13687,36 @@
       <c r="O273" s="4"/>
     </row>
     <row r="274" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A274" s="4"/>
-      <c r="B274" s="4"/>
-      <c r="C274" s="4"/>
-      <c r="D274" s="4"/>
-      <c r="E274" s="4"/>
-      <c r="F274" s="4"/>
-      <c r="G274" s="4"/>
-      <c r="H274" s="4"/>
-      <c r="I274" s="4"/>
-      <c r="J274" s="4"/>
+      <c r="A274" s="13">
+        <v>45469.604460856484</v>
+      </c>
+      <c r="B274" s="11" t="s">
+        <v>987</v>
+      </c>
+      <c r="C274" s="11" t="s">
+        <v>988</v>
+      </c>
+      <c r="D274" s="11">
+        <v>5952595</v>
+      </c>
+      <c r="E274" s="12" t="s">
+        <v>989</v>
+      </c>
+      <c r="F274" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G274" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H274" s="11" t="s">
+        <v>967</v>
+      </c>
+      <c r="I274" s="11" t="s">
+        <v>990</v>
+      </c>
+      <c r="J274" t="s">
+        <v>494</v>
+      </c>
       <c r="K274" s="4"/>
       <c r="L274" s="4"/>
       <c r="M274" s="4"/>
@@ -12921,16 +13724,36 @@
       <c r="O274" s="4"/>
     </row>
     <row r="275" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A275" s="4"/>
-      <c r="B275" s="4"/>
-      <c r="C275" s="4"/>
-      <c r="D275" s="4"/>
-      <c r="E275" s="4"/>
-      <c r="F275" s="4"/>
-      <c r="G275" s="4"/>
-      <c r="H275" s="4"/>
-      <c r="I275" s="4"/>
-      <c r="J275" s="4"/>
+      <c r="A275" s="13">
+        <v>45469.606514386571</v>
+      </c>
+      <c r="B275" s="11" t="s">
+        <v>991</v>
+      </c>
+      <c r="C275" s="11" t="s">
+        <v>992</v>
+      </c>
+      <c r="D275" s="11">
+        <v>5866755</v>
+      </c>
+      <c r="E275" s="11">
+        <v>11586035410</v>
+      </c>
+      <c r="F275" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G275" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H275" s="11" t="s">
+        <v>993</v>
+      </c>
+      <c r="I275" s="11" t="s">
+        <v>994</v>
+      </c>
+      <c r="J275" t="s">
+        <v>494</v>
+      </c>
       <c r="K275" s="4"/>
       <c r="L275" s="4"/>
       <c r="M275" s="4"/>
@@ -12938,16 +13761,36 @@
       <c r="O275" s="4"/>
     </row>
     <row r="276" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A276" s="4"/>
-      <c r="B276" s="4"/>
-      <c r="C276" s="4"/>
-      <c r="D276" s="4"/>
-      <c r="E276" s="4"/>
-      <c r="F276" s="4"/>
-      <c r="G276" s="4"/>
-      <c r="H276" s="4"/>
-      <c r="I276" s="4"/>
-      <c r="J276" s="4"/>
+      <c r="A276" s="13">
+        <v>45469.616124988424</v>
+      </c>
+      <c r="B276" s="11" t="s">
+        <v>995</v>
+      </c>
+      <c r="C276" s="11" t="s">
+        <v>996</v>
+      </c>
+      <c r="D276" s="11">
+        <v>5913821</v>
+      </c>
+      <c r="E276" s="11">
+        <v>60878991204</v>
+      </c>
+      <c r="F276" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G276" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H276" s="11" t="s">
+        <v>967</v>
+      </c>
+      <c r="I276" s="11" t="s">
+        <v>997</v>
+      </c>
+      <c r="J276" t="s">
+        <v>494</v>
+      </c>
       <c r="K276" s="4"/>
       <c r="L276" s="4"/>
       <c r="M276" s="4"/>
@@ -12955,16 +13798,36 @@
       <c r="O276" s="4"/>
     </row>
     <row r="277" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A277" s="4"/>
-      <c r="B277" s="4"/>
-      <c r="C277" s="4"/>
-      <c r="D277" s="4"/>
-      <c r="E277" s="4"/>
-      <c r="F277" s="4"/>
-      <c r="G277" s="4"/>
-      <c r="H277" s="4"/>
-      <c r="I277" s="4"/>
-      <c r="J277" s="4"/>
+      <c r="A277" s="13">
+        <v>45469.824185196761</v>
+      </c>
+      <c r="B277" s="11" t="s">
+        <v>998</v>
+      </c>
+      <c r="C277" s="11" t="s">
+        <v>999</v>
+      </c>
+      <c r="D277" s="11">
+        <v>5940339</v>
+      </c>
+      <c r="E277" s="11">
+        <v>12591647720</v>
+      </c>
+      <c r="F277" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G277" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H277" s="11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I277" s="11" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J277" t="s">
+        <v>494</v>
+      </c>
       <c r="K277" s="4"/>
       <c r="L277" s="4"/>
       <c r="M277" s="4"/>
@@ -12972,16 +13835,36 @@
       <c r="O277" s="4"/>
     </row>
     <row r="278" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A278" s="4"/>
-      <c r="B278" s="4"/>
-      <c r="C278" s="4"/>
-      <c r="D278" s="4"/>
-      <c r="E278" s="4"/>
-      <c r="F278" s="4"/>
-      <c r="G278" s="4"/>
-      <c r="H278" s="4"/>
-      <c r="I278" s="4"/>
-      <c r="J278" s="4"/>
+      <c r="A278" s="13">
+        <v>45470.414440451394</v>
+      </c>
+      <c r="B278" s="11" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C278" s="11" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D278" s="11">
+        <v>5979733</v>
+      </c>
+      <c r="E278" s="12" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F278" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G278" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H278" s="11" t="s">
+        <v>1005</v>
+      </c>
+      <c r="I278" s="11" t="s">
+        <v>1006</v>
+      </c>
+      <c r="J278" t="s">
+        <v>494</v>
+      </c>
       <c r="K278" s="4"/>
       <c r="L278" s="4"/>
       <c r="M278" s="4"/>
@@ -12989,38 +13872,148 @@
       <c r="O278" s="4"/>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A279" s="4"/>
-      <c r="B279" s="4"/>
-      <c r="C279" s="4"/>
-      <c r="D279" s="4"/>
-      <c r="E279" s="4"/>
-      <c r="F279" s="4"/>
-      <c r="G279" s="4"/>
-      <c r="H279" s="4"/>
-      <c r="I279" s="4"/>
-      <c r="J279" s="4"/>
+      <c r="A279" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C279" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D279" s="4">
+        <v>5966974</v>
+      </c>
+      <c r="E279" s="4">
+        <v>2524793354</v>
+      </c>
+      <c r="F279" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G279" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H279" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I279" s="4" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J279" s="4" t="s">
+        <v>494</v>
+      </c>
       <c r="K279" s="4"/>
       <c r="L279" s="4"/>
       <c r="M279" s="4"/>
       <c r="N279" s="4"/>
       <c r="O279" s="4"/>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A280" s="4"/>
-      <c r="B280" s="4"/>
-      <c r="C280" s="4"/>
-      <c r="D280" s="4"/>
-      <c r="E280" s="4"/>
-      <c r="F280" s="4"/>
-      <c r="G280" s="4"/>
-      <c r="H280" s="4"/>
-      <c r="I280" s="4"/>
-      <c r="J280" s="4"/>
-      <c r="K280" s="4"/>
-      <c r="L280" s="4"/>
-      <c r="M280" s="4"/>
-      <c r="N280" s="4"/>
-      <c r="O280" s="4"/>
+    <row r="280" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="13" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B280" s="11" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C280" s="11" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D280" s="11">
+        <v>5966485</v>
+      </c>
+      <c r="E280" s="12">
+        <v>45029371850</v>
+      </c>
+      <c r="F280" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G280" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H280" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I280" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J280" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="281" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B281" s="11" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C281" s="11" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D281" s="11">
+        <v>5966611</v>
+      </c>
+      <c r="E281" s="11">
+        <v>793996309</v>
+      </c>
+      <c r="F281" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G281" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H281" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I281" s="11" t="s">
+        <v>1013</v>
+      </c>
+      <c r="J281" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="282" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="19" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D282">
+        <v>5966566</v>
+      </c>
+      <c r="E282">
+        <v>12424148600</v>
+      </c>
+      <c r="F282" t="s">
+        <v>40</v>
+      </c>
+      <c r="G282" t="s">
+        <v>12</v>
+      </c>
+      <c r="H282" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I282" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J282" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="283" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="13"/>
+      <c r="B283" s="11"/>
+      <c r="C283" s="11"/>
+      <c r="D283" s="11"/>
+      <c r="E283" s="12"/>
+      <c r="F283" s="11"/>
+      <c r="G283" s="11"/>
+      <c r="H283" s="11"/>
+      <c r="I283" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J206" xr:uid="{91F6D7D1-5711-44E6-A7F2-3BDEABEFDFB8}"/>
@@ -13029,5 +14022,6 @@
     <hyperlink ref="I20" r:id="rId2" xr:uid="{88D78E84-C428-4CC3-813B-77D74E74CBBA}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
botao de recuperação ajuste
</commit_message>
<xml_diff>
--- a/cad_user/USUARIOS CONFIRMADOS IMEIGUARD.xlsx
+++ b/cad_user/USUARIOS CONFIRMADOS IMEIGUARD.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DEAC_TI_SW\Users\DEAC_TI_SERVER\Desktop\IMEIGUARD\cad_user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imeiguard\cad_user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395D0C1E-12E8-4CCC-94C4-47543FD548A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6C345-87D3-450C-B7D0-F72AA53ACF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D5B3F50-1031-4000-A71D-A098494E9EE1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D5B3F50-1031-4000-A71D-A098494E9EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$J$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$J$324</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="1170">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -3366,6 +3366,189 @@
   </si>
   <si>
     <t>JONHNATAN WALACE MEIRELES</t>
+  </si>
+  <si>
+    <t>andressasilvapla@gmail.com</t>
+  </si>
+  <si>
+    <t>ANDRESSA DOS SANTOS SILVA</t>
+  </si>
+  <si>
+    <t>Andressa.santos@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>joycebohn89@gmail.com</t>
+  </si>
+  <si>
+    <t>JOYCE MAIKA BOHN</t>
+  </si>
+  <si>
+    <t>DELEGACIA DO ICUI-GUAJARA</t>
+  </si>
+  <si>
+    <t>joyce_bohn@hotmail.com</t>
+  </si>
+  <si>
+    <t>paulosouza4090@gmail.com</t>
+  </si>
+  <si>
+    <t>paulo.benjamim@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>gisely.sousa16@gmail.com</t>
+  </si>
+  <si>
+    <t>DPID</t>
+  </si>
+  <si>
+    <t>DEAM/DEACA BRAGANCA</t>
+  </si>
+  <si>
+    <t>PAULO BENJAMIM DE SOUZA</t>
+  </si>
+  <si>
+    <t>GISELY PENICHE DA SILVA SOUSA</t>
+  </si>
+  <si>
+    <t>marcelofernando2322@gmail.com</t>
+  </si>
+  <si>
+    <t>edinildojunior@hotmail.com</t>
+  </si>
+  <si>
+    <t>EDINILDO DE MENEZES COSTA JUNIOR</t>
+  </si>
+  <si>
+    <t>edinildo.junior@policiacivil.pa.gov.br</t>
+  </si>
+  <si>
+    <t>igorpersonal19@gmail.com</t>
+  </si>
+  <si>
+    <t>IGOR MARCIO BATISTA SERAFIM</t>
+  </si>
+  <si>
+    <t>3º BME / CASTANHAL</t>
+  </si>
+  <si>
+    <t>romulloneri@gmail.com</t>
+  </si>
+  <si>
+    <t>14°BPM</t>
+  </si>
+  <si>
+    <t>ericknunesn@gmail.com</t>
+  </si>
+  <si>
+    <t>ERICK NUNES PRASERES</t>
+  </si>
+  <si>
+    <t>ERICKNUNESN@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>thiagosousa.ts548@gmail.com</t>
+  </si>
+  <si>
+    <t>14° BPM</t>
+  </si>
+  <si>
+    <t>MARCELO FERNANDO VASCONCELOS CUNHA</t>
+  </si>
+  <si>
+    <t>ROMULO TIAGO PANTOJA NERI</t>
+  </si>
+  <si>
+    <t>THIAGO DE SOUZA MORAES</t>
+  </si>
+  <si>
+    <t>9 SECCIONAL DE MOSQUEIRO/PA</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE POLICIA CIVIL DE VILA DOS CABANOS</t>
+  </si>
+  <si>
+    <t>14⁰ BATALHAO</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>caveira39pmpa@gmail.com</t>
+  </si>
+  <si>
+    <t>3⁰ BME</t>
+  </si>
+  <si>
+    <t>yuripmpa2014@gmail.com</t>
+  </si>
+  <si>
+    <t>rafaelgc.rg@gmail.com</t>
+  </si>
+  <si>
+    <t>3 BME CASTANHAL</t>
+  </si>
+  <si>
+    <t>cbodair30@gmail.com</t>
+  </si>
+  <si>
+    <t>3° BME</t>
+  </si>
+  <si>
+    <t>justinoamaral74@gmail.com</t>
+  </si>
+  <si>
+    <t>sdrenato2014@gmail.com</t>
+  </si>
+  <si>
+    <t>3° BME CASTANHAL</t>
+  </si>
+  <si>
+    <t>hanna.salesp@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CLEOMAR MATOS COSTA</t>
+  </si>
+  <si>
+    <t>YURI KELLYSSON BEZERRA DE ARAUJO</t>
+  </si>
+  <si>
+    <t>RAFAEL GARCIA CHAVES</t>
+  </si>
+  <si>
+    <t>ODAIR JOSE CARNEIRO PEREIRA</t>
+  </si>
+  <si>
+    <t>JUSTINO AMARAL DE SOUZA</t>
+  </si>
+  <si>
+    <t>JOAO RENATO DE LIMA</t>
+  </si>
+  <si>
+    <t>HANNA PAULA SALES PAIVA</t>
+  </si>
+  <si>
+    <t>3° BATALHAO DE MISSOES ESPECIAIS</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>thicianneferreira10@gmail.com</t>
+  </si>
+  <si>
+    <t>eduespirito@hotmail.com</t>
+  </si>
+  <si>
+    <t>EDUARDO RODRIGUES DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>THICIANNE PATRICIA PORTELA FERREIRA</t>
+  </si>
+  <si>
+    <t>DELEGACIA DE CAPITÃO POÇO</t>
   </si>
 </sst>
 </file>
@@ -3416,6 +3599,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3904,20 +4088,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F6D7D1-5711-44E6-A7F2-3BDEABEFDFB8}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:O307"/>
+  <dimension ref="A1:O326"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A307" sqref="A307:J307"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A325" sqref="A325:J326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="5"/>
-    <col min="2" max="2" width="35.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="20.7109375" style="5"/>
-    <col min="8" max="8" width="67.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="43.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="20.7109375" style="5"/>
   </cols>
@@ -14494,7 +14678,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="289" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="25">
         <v>45484.618807870371</v>
       </c>
@@ -14718,7 +14902,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="25">
         <v>45484.886273148149</v>
       </c>
@@ -14787,7 +14971,7 @@
         <v>45485.945833333331</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>1077</v>
+        <v>1155</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>1078</v>
@@ -14879,162 +15063,162 @@
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" s="23">
+      <c r="A301" s="30">
         <v>45489.523611111108</v>
       </c>
-      <c r="B301" s="24" t="s">
+      <c r="B301" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="C301" s="24" t="s">
+      <c r="C301" s="5" t="s">
         <v>1089</v>
       </c>
-      <c r="D301" s="24">
+      <c r="D301" s="5">
         <v>5331501</v>
       </c>
-      <c r="E301" s="24">
+      <c r="E301" s="5">
         <v>21852170204</v>
       </c>
-      <c r="F301" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G301" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H301" s="24" t="s">
+      <c r="F301" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G301" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H301" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="I301" s="24" t="s">
+      <c r="I301" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="J301" s="24" t="s">
+      <c r="J301" s="5" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A302" s="23">
+      <c r="A302" s="30">
         <v>45489.581250000003</v>
       </c>
-      <c r="B302" s="24" t="s">
+      <c r="B302" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="C302" s="24" t="s">
+      <c r="C302" s="5" t="s">
         <v>1092</v>
       </c>
-      <c r="D302" s="24">
+      <c r="D302" s="5">
         <v>5940474</v>
       </c>
-      <c r="E302" s="24">
+      <c r="E302" s="5">
         <v>2060056012</v>
       </c>
-      <c r="F302" s="24" t="s">
+      <c r="F302" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G302" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H302" s="24" t="s">
+      <c r="G302" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H302" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="I302" s="24" t="s">
+      <c r="I302" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="J302" s="24" t="s">
+      <c r="J302" s="5" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A303" s="23">
+      <c r="A303" s="30">
         <v>45489.725694444445</v>
       </c>
-      <c r="B303" s="24" t="s">
+      <c r="B303" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="C303" s="24" t="s">
+      <c r="C303" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="D303" s="24">
+      <c r="D303" s="5">
         <v>5913936</v>
       </c>
-      <c r="E303" s="24">
+      <c r="E303" s="5">
         <v>3295607435</v>
       </c>
-      <c r="F303" s="24" t="s">
+      <c r="F303" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G303" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H303" s="24" t="s">
+      <c r="G303" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H303" s="5" t="s">
         <v>1094</v>
       </c>
-      <c r="I303" s="24" t="s">
+      <c r="I303" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="J303" s="24" t="s">
+      <c r="J303" s="5" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A304" s="23">
+      <c r="A304" s="30">
         <v>45490.347222222219</v>
       </c>
-      <c r="B304" s="24" t="s">
+      <c r="B304" s="5" t="s">
         <v>1095</v>
       </c>
-      <c r="C304" s="24" t="s">
+      <c r="C304" s="5" t="s">
         <v>1096</v>
       </c>
-      <c r="D304" s="24">
+      <c r="D304" s="5">
         <v>5967000</v>
       </c>
-      <c r="E304" s="24">
+      <c r="E304" s="5">
         <v>17348017889</v>
       </c>
-      <c r="F304" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G304" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H304" s="24" t="s">
+      <c r="F304" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G304" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H304" s="5" t="s">
         <v>1097</v>
       </c>
-      <c r="I304" s="24" t="s">
+      <c r="I304" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="J304" s="24" t="s">
+      <c r="J304" s="5" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="305" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="23">
+      <c r="A305" s="30">
         <v>45490.467361111114</v>
       </c>
-      <c r="B305" s="24" t="s">
+      <c r="B305" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="C305" s="24" t="s">
+      <c r="C305" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="D305" s="24">
+      <c r="D305" s="5">
         <v>5966792</v>
       </c>
-      <c r="E305" s="24">
+      <c r="E305" s="5">
         <v>4671853361</v>
       </c>
-      <c r="F305" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G305" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H305" s="24" t="s">
+      <c r="F305" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G305" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H305" s="5" t="s">
         <v>1086</v>
       </c>
-      <c r="I305" s="24" t="s">
+      <c r="I305" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="J305" s="24" t="s">
+      <c r="J305" s="5" t="s">
         <v>494</v>
       </c>
     </row>
@@ -15098,12 +15282,620 @@
       <c r="I307" s="21" t="s">
         <v>1105</v>
       </c>
-      <c r="J307" s="24" t="s">
+      <c r="J307" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" s="30">
+        <v>45496.618055555555</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C308" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D308" s="5">
+        <v>5967004</v>
+      </c>
+      <c r="E308" s="5">
+        <v>2540968244</v>
+      </c>
+      <c r="F308" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G308" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H308" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="I308" s="5" t="s">
+        <v>1111</v>
+      </c>
+      <c r="J308" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="30">
+        <v>45496.790972222225</v>
+      </c>
+      <c r="B309" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C309" s="5" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D309" s="5">
+        <v>5940092</v>
+      </c>
+      <c r="E309" s="5">
+        <v>93534507215</v>
+      </c>
+      <c r="F309" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G309" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H309" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I309" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J309" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="20">
+        <v>45500.525150462963</v>
+      </c>
+      <c r="B310" s="21" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C310" s="21" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D310" s="22">
+        <v>5966272</v>
+      </c>
+      <c r="E310" s="21">
+        <v>1223439216</v>
+      </c>
+      <c r="F310" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G310" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H310" s="21" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I310" s="21" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J310" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="20">
+        <v>45500.528819444444</v>
+      </c>
+      <c r="B311" s="21" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C311" s="21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D311" s="22">
+        <v>5942641</v>
+      </c>
+      <c r="E311" s="21">
+        <v>870925229</v>
+      </c>
+      <c r="F311" s="21" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G311" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H311" s="21" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I311" s="21" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J311" s="4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="20">
+        <v>45503.643055555556</v>
+      </c>
+      <c r="B312" s="21" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C312" s="21" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D312" s="22">
+        <v>5482879</v>
+      </c>
+      <c r="E312" s="22">
+        <v>30576571253</v>
+      </c>
+      <c r="F312" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G312" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H312" s="21" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I312" s="21" t="s">
+        <v>1123</v>
+      </c>
+      <c r="J312" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A313" s="20">
+        <v>45503.701041666667</v>
+      </c>
+      <c r="B313" s="21" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C313" s="21" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D313" s="22">
+        <v>5975449</v>
+      </c>
+      <c r="E313" s="21">
+        <v>4587204374</v>
+      </c>
+      <c r="F313" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G313" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H313" s="21" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I313" s="21" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J313" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="20">
+        <v>45504.47693287037</v>
+      </c>
+      <c r="B314" s="21" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C314" s="21" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D314" s="22">
+        <v>4220564</v>
+      </c>
+      <c r="E314" s="21">
+        <v>1140953290</v>
+      </c>
+      <c r="F314" s="21" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G314" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H314" s="21" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I314" s="21" t="s">
+        <v>1127</v>
+      </c>
+      <c r="J314" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="20">
+        <v>45505.313726851855</v>
+      </c>
+      <c r="B315" s="21" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C315" s="21" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D315" s="21">
+        <v>6401542</v>
+      </c>
+      <c r="E315" s="21">
+        <v>84651849253</v>
+      </c>
+      <c r="F315" s="21" t="s">
+        <v>728</v>
+      </c>
+      <c r="G315" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H315" s="21" t="s">
+        <v>1131</v>
+      </c>
+      <c r="I315" s="21" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J315" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="20">
+        <v>45505.315347222226</v>
+      </c>
+      <c r="B316" s="21" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C316" s="21" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D316" s="21">
+        <v>3541170</v>
+      </c>
+      <c r="E316" s="21">
+        <v>2463425288</v>
+      </c>
+      <c r="F316" s="21" t="s">
+        <v>728</v>
+      </c>
+      <c r="G316" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H316" s="21" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I316" s="21" t="s">
+        <v>1134</v>
+      </c>
+      <c r="J316" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="20">
+        <v>45505.315451388888</v>
+      </c>
+      <c r="B317" s="21" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C317" s="21" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D317" s="22">
+        <v>3542370</v>
+      </c>
+      <c r="E317" s="21">
+        <v>5177578267</v>
+      </c>
+      <c r="F317" s="21" t="s">
+        <v>728</v>
+      </c>
+      <c r="G317" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H317" s="21" t="s">
+        <v>1136</v>
+      </c>
+      <c r="I317" s="21" t="s">
+        <v>1135</v>
+      </c>
+      <c r="J317" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="20">
+        <v>45505.591111111113</v>
+      </c>
+      <c r="B318" s="21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C318" s="21" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D318" s="21">
+        <v>54193346</v>
+      </c>
+      <c r="E318" s="22">
+        <v>64109232287</v>
+      </c>
+      <c r="F318" s="21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G318" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H318" s="21" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I318" s="21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="J318" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="20">
+        <v>45505.591898148145</v>
+      </c>
+      <c r="B319" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C319" s="21" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D319" s="22">
+        <v>39880</v>
+      </c>
+      <c r="E319" s="21">
+        <v>7264035476</v>
+      </c>
+      <c r="F319" s="21" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G319" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H319" s="21" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I319" s="21" t="s">
+        <v>1146</v>
+      </c>
+      <c r="J319" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A320" s="20">
+        <v>45505.592280092591</v>
+      </c>
+      <c r="B320" s="21" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C320" s="21" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D320" s="22">
+        <v>6402090</v>
+      </c>
+      <c r="E320" s="21">
+        <v>813542235</v>
+      </c>
+      <c r="F320" s="21" t="s">
+        <v>728</v>
+      </c>
+      <c r="G320" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H320" s="21" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I320" s="21" t="s">
+        <v>1147</v>
+      </c>
+      <c r="J320" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A321" s="20">
+        <v>45505.595949074072</v>
+      </c>
+      <c r="B321" s="21" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C321" s="21" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D321" s="22">
+        <v>5788900</v>
+      </c>
+      <c r="E321" s="22">
+        <v>38038498291</v>
+      </c>
+      <c r="F321" s="21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G321" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H321" s="21" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I321" s="21" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J321" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A322" s="20">
+        <v>45505.702696759261</v>
+      </c>
+      <c r="B322" s="21" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C322" s="21" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D322" s="22">
+        <v>5789001</v>
+      </c>
+      <c r="E322" s="22">
+        <v>39548651220</v>
+      </c>
+      <c r="F322" s="21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G322" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H322" s="21" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I322" s="21" t="s">
+        <v>1151</v>
+      </c>
+      <c r="J322" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A323" s="20">
+        <v>45506.661620370367</v>
+      </c>
+      <c r="B323" s="21" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C323" s="21" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D323" s="21">
+        <v>4218867</v>
+      </c>
+      <c r="E323" s="22">
+        <v>89038827253</v>
+      </c>
+      <c r="F323" s="21" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G323" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H323" s="21" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I323" s="21" t="s">
+        <v>1152</v>
+      </c>
+      <c r="J323" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="20">
+        <v>45507.370185185187</v>
+      </c>
+      <c r="B324" s="21" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C324" s="21" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D324" s="22">
+        <v>5966676</v>
+      </c>
+      <c r="E324" s="22">
+        <v>96565470200</v>
+      </c>
+      <c r="F324" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G324" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H324" s="21" t="s">
+        <v>893</v>
+      </c>
+      <c r="I324" s="21" t="s">
+        <v>1154</v>
+      </c>
+      <c r="J324" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="20">
+        <v>45512.697615740741</v>
+      </c>
+      <c r="B325" s="21" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C325" s="21" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D325" s="22">
+        <v>5966996</v>
+      </c>
+      <c r="E325" s="21">
+        <v>1812903324</v>
+      </c>
+      <c r="F325" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G325" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H325" s="21" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I325" s="21" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J325" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="20">
+        <v>45512.698645833334</v>
+      </c>
+      <c r="B326" s="21" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C326" s="21" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D326" s="22">
+        <v>56927251</v>
+      </c>
+      <c r="E326" s="22">
+        <v>35721944234</v>
+      </c>
+      <c r="F326" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G326" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H326" s="21" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I326" s="21" t="s">
+        <v>1166</v>
+      </c>
+      <c r="J326" s="5" t="s">
         <v>494</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J206" xr:uid="{91F6D7D1-5711-44E6-A7F2-3BDEABEFDFB8}"/>
+  <autoFilter ref="A1:J324" xr:uid="{91F6D7D1-5711-44E6-A7F2-3BDEABEFDFB8}"/>
   <hyperlinks>
     <hyperlink ref="I94" r:id="rId1" xr:uid="{F5781726-80CC-438F-B4F1-91CB3DEF0F75}"/>
     <hyperlink ref="I20" r:id="rId2" xr:uid="{88D78E84-C428-4CC3-813B-77D74E74CBBA}"/>

</xml_diff>